<commit_message>
Add standoffs to BOM
</commit_message>
<xml_diff>
--- a/Two Armed Bandit BOM.xlsx
+++ b/Two Armed Bandit BOM.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ofer/Instrumentation/Projects/Michael Wallace PCB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ofer/Dropbox (HMS)/RIC/Projects/Michael Wallace Two Armed Bandit PCB/PCB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4782C2CF-EC12-F546-A5CC-477A3B2DDD1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5292CF62-CA05-7749-8652-DE287E06DDD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{0B0E9FC3-E6BF-9040-85FC-13E82E5FB543}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t>Two Armed Bandit PCB</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>get 40-pin header and break to size</t>
+  </si>
+  <si>
+    <t>McMaster</t>
+  </si>
+  <si>
+    <t>92745A326</t>
   </si>
 </sst>
 </file>
@@ -567,7 +573,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -667,7 +673,7 @@
         <v>2.15</v>
       </c>
       <c r="H7" s="4">
-        <f t="shared" ref="H7:H20" si="0">G7*D7</f>
+        <f t="shared" ref="H7:H22" si="0">G7*D7</f>
         <v>2.15</v>
       </c>
       <c r="J7" s="1" t="s">
@@ -920,9 +926,31 @@
         <v>0</v>
       </c>
     </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H21" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>44</v>
+      </c>
+      <c r="D22" s="1">
+        <v>4</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0.46</v>
+      </c>
+      <c r="H22" s="4">
+        <f t="shared" si="0"/>
+        <v>1.84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update BOM for MTA-100 connectors
</commit_message>
<xml_diff>
--- a/Two Armed Bandit BOM.xlsx
+++ b/Two Armed Bandit BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ofer/Dropbox (HMS)/RIC/Projects/Michael Wallace Two Armed Bandit PCB/PCB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5292CF62-CA05-7749-8652-DE287E06DDD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E4C8A1-72DD-374B-9088-52ADBB27089A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{0B0E9FC3-E6BF-9040-85FC-13E82E5FB543}"/>
+    <workbookView xWindow="6860" yWindow="2700" windowWidth="25600" windowHeight="15540" xr2:uid="{0B0E9FC3-E6BF-9040-85FC-13E82E5FB543}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
   <si>
     <t>Two Armed Bandit PCB</t>
   </si>
@@ -146,21 +146,9 @@
     <t>Alternatively: WM7862-ND</t>
   </si>
   <si>
-    <t>2-pin socket</t>
-  </si>
-  <si>
-    <t>3-pin socket</t>
-  </si>
-  <si>
     <t>8-pin socket</t>
   </si>
   <si>
-    <t>S7036-ND</t>
-  </si>
-  <si>
-    <t>S7035-ND</t>
-  </si>
-  <si>
     <t>S7041-ND</t>
   </si>
   <si>
@@ -198,6 +186,45 @@
   </si>
   <si>
     <t>92745A326</t>
+  </si>
+  <si>
+    <t>A19423-ND</t>
+  </si>
+  <si>
+    <t>A19430-ND</t>
+  </si>
+  <si>
+    <t>3-pin header (MTA-100)</t>
+  </si>
+  <si>
+    <t>2-pin header (MTA-100)</t>
+  </si>
+  <si>
+    <t>Or any other suitable connector</t>
+  </si>
+  <si>
+    <t>2-pin MTA-100 connector (for ribbon)</t>
+  </si>
+  <si>
+    <t>3-pin MTA-100 connector (for ribbon)</t>
+  </si>
+  <si>
+    <t>A31080-ND</t>
+  </si>
+  <si>
+    <t>A31081-ND</t>
+  </si>
+  <si>
+    <t>MTA-100 Crimper (if needed)</t>
+  </si>
+  <si>
+    <t>58579-1</t>
+  </si>
+  <si>
+    <t>For Ribbon Cable Connectors:</t>
+  </si>
+  <si>
+    <t>Can be found at Digikey, Newark, Amazon, or direct from TE connectivity</t>
   </si>
 </sst>
 </file>
@@ -569,11 +596,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB9E1C0-7D08-FB49-A5D8-A9FD30E849E1}">
-  <dimension ref="B2:J22"/>
+  <dimension ref="B2:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -584,7 +611,8 @@
     <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="22" style="1" customWidth="1"/>
-    <col min="7" max="8" width="10.83203125" style="4"/>
+    <col min="7" max="7" width="11.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="4"/>
     <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -673,7 +701,7 @@
         <v>2.15</v>
       </c>
       <c r="H7" s="4">
-        <f t="shared" ref="H7:H22" si="0">G7*D7</f>
+        <f t="shared" ref="H7:H27" si="0">G7*D7</f>
         <v>2.15</v>
       </c>
       <c r="J7" s="1" t="s">
@@ -685,20 +713,23 @@
         <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="D8" s="1">
         <v>6</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="G8" s="4">
-        <v>0.33</v>
+        <v>0.1</v>
       </c>
       <c r="H8" s="4">
         <f t="shared" si="0"/>
-        <v>1.98</v>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -706,20 +737,23 @@
         <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="D9" s="1">
         <v>3</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="G9" s="4">
-        <v>0.35</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H9" s="4">
         <f t="shared" si="0"/>
-        <v>1.0499999999999998</v>
+        <v>0.42000000000000004</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
@@ -739,7 +773,7 @@
         <v>3.26</v>
       </c>
       <c r="H10" s="4">
-        <f>G10*D20</f>
+        <f>G10*D25</f>
         <v>3.26</v>
       </c>
       <c r="J10" s="1" t="s">
@@ -775,13 +809,13 @@
         <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G12" s="4">
         <v>0.67</v>
@@ -817,7 +851,7 @@
         <v>25</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D14" s="1">
         <v>3</v>
@@ -844,16 +878,16 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G16" s="4">
         <v>0.51</v>
@@ -863,92 +897,121 @@
         <v>0.51</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H17" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H18" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H19" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="1">
-        <v>1</v>
-      </c>
-      <c r="H20" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H21" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="C21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0.15</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="1">
+        <v>57</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" s="4">
+        <v>400</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="H25" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="1">
         <v>4</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G22" s="4">
+      <c r="E27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G27" s="4">
         <v>0.46</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H27" s="4">
         <f t="shared" si="0"/>
         <v>1.84</v>
       </c>

</xml_diff>